<commit_message>
fix: Complete time units conversion from hours to days
- Fix all remaining flux units: mM/h → mM/day
- Fix all hovertemplates: h → days
- Fix all axis labels in flux, bohr, and sensitivity plots
- Fix flux statistics table units
- Update docstrings
- Complete consistency across entire application
</commit_message>
<xml_diff>
--- a/Data_Brodbar_et_al_exp.xlsx
+++ b/Data_Brodbar_et_al_exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorgelindo\Desktop\Mario_RBC_up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D92D490-0579-4BF3-A3F5-C4FDA9F36AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D294F3E9-588B-4887-8D81-92D6FA042D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1008" windowWidth="23232" windowHeight="12576" xr2:uid="{972B49CD-1A65-4198-84D7-F25D33329B6E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{972B49CD-1A65-4198-84D7-F25D33329B6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2609,10 +2609,13 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>